<commit_message>
15th May Daily Stand-Up meeting minutes and updated burndown chart
- Meeting minutes for 15th May daily standup have been uploaded
- Burndown chart updated as one user story has been moved into done column
</commit_message>
<xml_diff>
--- a/Documentation - Sprint 1/Rush Racing Sprint 1 Burndown Chart.xlsx
+++ b/Documentation - Sprint 1/Rush Racing Sprint 1 Burndown Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Papaya\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Papaya\Documents\REPOS\Rush Racing Repo\Rush-Racing\Documentation - Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4FF99C-EBEE-427C-BC2C-95291F9AFFEF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36468B2-B510-45D3-B278-063A39F0889C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 Burndown Chart" sheetId="2" r:id="rId1"/>
@@ -550,22 +550,22 @@
                   <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>73</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>73</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>73</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>73</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>73</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>73</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1970,8 +1970,8 @@
   <dimension ref="A1:AF41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2487,22 +2487,22 @@
         <v>5</v>
       </c>
       <c r="M11" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N11" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O11" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P11" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R11" s="23">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:32" s="2" customFormat="1" ht="30" customHeight="1">
@@ -2767,7 +2767,7 @@
         <v>73</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" ref="C17:R17" si="0">SUM(F4:F16)</f>
+        <f t="shared" ref="F17:R17" si="0">SUM(F4:F16)</f>
         <v>73</v>
       </c>
       <c r="G17" s="1">
@@ -2796,27 +2796,27 @@
       </c>
       <c r="M17" s="1">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="N17" s="1">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="O17" s="1">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="P17" s="1">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="Q17" s="1">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="R17" s="1">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="S17" s="17"/>
     </row>
@@ -2834,7 +2834,7 @@
         <v>68.13333333333334</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" ref="C18:R18" si="1">$A$22-E3*$A$22/$B$22</f>
+        <f t="shared" ref="E18:R18" si="1">$A$22-E3*$A$22/$B$22</f>
         <v>63.266666666666666</v>
       </c>
       <c r="F18" s="3">
@@ -3191,7 +3191,7 @@
     <row r="32" spans="1:19" s="2" customFormat="1">
       <c r="A32" s="7">
         <f xml:space="preserve"> M17</f>
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B32" s="5">
         <v>5</v>
@@ -3216,7 +3216,7 @@
     <row r="33" spans="1:18" s="2" customFormat="1">
       <c r="A33" s="7">
         <f xml:space="preserve"> N17</f>
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B33" s="5">
         <v>4</v>
@@ -3241,7 +3241,7 @@
     <row r="34" spans="1:18" s="2" customFormat="1">
       <c r="A34" s="7">
         <f xml:space="preserve"> O17</f>
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B34" s="5">
         <v>3</v>
@@ -3266,7 +3266,7 @@
     <row r="35" spans="1:18" s="2" customFormat="1">
       <c r="A35" s="7">
         <f xml:space="preserve"> P17</f>
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B35" s="5">
         <v>2</v>
@@ -3291,7 +3291,7 @@
     <row r="36" spans="1:18" s="2" customFormat="1">
       <c r="A36" s="7">
         <f xml:space="preserve"> Q17</f>
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B36" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
Update Rush Racing Sprint 1 Burndown Chart.xlsx
Updated burn down chart with completed user story points deducted
</commit_message>
<xml_diff>
--- a/Documentation - Sprint 1/Rush Racing Sprint 1 Burndown Chart.xlsx
+++ b/Documentation - Sprint 1/Rush Racing Sprint 1 Burndown Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Papaya\Documents\REPOS\Rush Racing Repo\Rush-Racing\Documentation - Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36468B2-B510-45D3-B278-063A39F0889C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480ABFC7-7E49-4F44-AC28-EB2D5240FBF3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="225" yWindow="8700" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 Burndown Chart" sheetId="2" r:id="rId1"/>
@@ -553,19 +553,19 @@
                   <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>68</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>68</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>68</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>68</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>68</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1971,7 +1971,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T22" sqref="T22"/>
+      <selection pane="bottomLeft" activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2098,19 +2098,19 @@
         <v>1</v>
       </c>
       <c r="N4" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:32" s="2" customFormat="1" ht="30" customHeight="1">
@@ -2658,19 +2658,19 @@
         <v>13</v>
       </c>
       <c r="N14" s="15">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="O14" s="15">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="P14" s="15">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="15">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="R14" s="23">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:32" s="2" customFormat="1" ht="30.75" thickBot="1">
@@ -2800,23 +2800,23 @@
       </c>
       <c r="N17" s="1">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="O17" s="1">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="P17" s="1">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="Q17" s="1">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="R17" s="1">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="S17" s="17"/>
     </row>
@@ -3216,7 +3216,7 @@
     <row r="33" spans="1:18" s="2" customFormat="1">
       <c r="A33" s="7">
         <f xml:space="preserve"> N17</f>
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B33" s="5">
         <v>4</v>
@@ -3241,7 +3241,7 @@
     <row r="34" spans="1:18" s="2" customFormat="1">
       <c r="A34" s="7">
         <f xml:space="preserve"> O17</f>
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B34" s="5">
         <v>3</v>
@@ -3266,7 +3266,7 @@
     <row r="35" spans="1:18" s="2" customFormat="1">
       <c r="A35" s="7">
         <f xml:space="preserve"> P17</f>
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B35" s="5">
         <v>2</v>
@@ -3291,7 +3291,7 @@
     <row r="36" spans="1:18" s="2" customFormat="1">
       <c r="A36" s="7">
         <f xml:space="preserve"> Q17</f>
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B36" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
Various changes, added unit testing scripts
- Finished unit testing script CurrencyTest
- Various fixes and changes
- Added a terrain on the lambo track so users do not fall off the track
</commit_message>
<xml_diff>
--- a/Documentation - Sprint 1/Rush Racing Sprint 1 Burndown Chart.xlsx
+++ b/Documentation - Sprint 1/Rush Racing Sprint 1 Burndown Chart.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Papaya\Documents\REPOS\Rush Racing Repo\Rush-Racing\Documentation - Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB6729E-2943-4589-BF30-7D51CC013A1F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE41786-5E3A-4D75-AC01-0BF2B1DBF9CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4170" yWindow="2175" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 Burndown Chart" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sprint 1 Burndown Chart'!$A$1:$S$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sprint 1 Burndown Chart'!$A$1:$AC$38</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -565,7 +565,7 @@
                   <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>49</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1701,6 +1701,115 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>13607</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>13606</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3619499" cy="7075715"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1413675-B845-4C07-A755-58ACC2EFAF9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10967357" y="1537606"/>
+          <a:ext cx="3619499" cy="7075715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1600" b="1"/>
+            <a:t>Reflection</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1600" b="1" baseline="0"/>
+            <a:t> of p</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1600" b="1"/>
+            <a:t>rogress of sprint 1 burndown chart:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1400"/>
+            <a:t>Our sprint 1 burndown chart is not as great as we expected.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-NZ" sz="1400" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1400" baseline="0"/>
+            <a:t>Firstly, we underestimated the time that project setup would take. The first week of development was spent setting up as well as ironing out any problems we had with Unity or Github. User story development could only be started around the end of the first week.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-NZ" sz="1400" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1400" baseline="0"/>
+            <a:t>Secondly, as the semester gets busier and other papers and assignments to juggle, testing user stories was low priority in some cases and testing was not complete as straight as user stories were moved into the testing column. Sometimes, we had to focus on getting our development user stories complete. </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-NZ" sz="1400" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1400" baseline="0"/>
+            <a:t>Thirdly, we have some user stories that were not complete that will be brought into sprint 2. That is why the burndown chart does not touch the ground.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-NZ" sz="1400" baseline="0"/>
+          </a:br>
+          <a:br>
+            <a:rPr lang="en-NZ" sz="1400" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1400" baseline="0"/>
+            <a:t>From next sprint, we are going to make sure to prioritise user story testing as soon as they are ready. This also involves better communication between the developer and tester to let each other know the status of user stories.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1400" baseline="0"/>
+            <a:t>With a better understanding of time estimation of development, we will ensure to practice better time management for this project and hopefully have a burndown chart that sticks closer to the ideal trend for sprint 2.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-NZ" sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1967,11 +2076,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AF41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T5" sqref="T5"/>
+      <selection pane="bottomLeft" activeCell="AG15" sqref="AG15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2222,7 +2334,7 @@
         <v>2</v>
       </c>
       <c r="R6" s="23">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:32" s="2" customFormat="1" ht="30" customHeight="1">
@@ -2390,7 +2502,7 @@
         <v>5</v>
       </c>
       <c r="R9" s="23">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:32" s="2" customFormat="1" ht="30" customHeight="1">
@@ -2446,7 +2558,7 @@
         <v>5</v>
       </c>
       <c r="R10" s="23">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:32" s="2" customFormat="1" ht="30" customHeight="1">
@@ -2726,7 +2838,7 @@
         <v>13</v>
       </c>
       <c r="R15" s="24">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:32" s="2" customFormat="1" ht="27" customHeight="1">
@@ -2816,7 +2928,7 @@
       </c>
       <c r="R17" s="1">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="S17" s="17"/>
     </row>
@@ -3415,7 +3527,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="19" max="36" man="1"/>
   </colBreaks>

</xml_diff>